<commit_message>
move addressing  mode registers to the end
</commit_message>
<xml_diff>
--- a/CPU.xlsx
+++ b/CPU.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -1018,7 +1018,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1080,6 +1080,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1418,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,7 +2452,7 @@
       <c r="K39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="38" t="s">
+      <c r="M39" s="39" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2476,7 +2479,7 @@
       <c r="J40" s="31"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="38"/>
+      <c r="M40" s="39"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -2501,7 +2504,7 @@
       <c r="J41" s="31"/>
       <c r="K41" s="2"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="38"/>
+      <c r="M41" s="39"/>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -2526,7 +2529,7 @@
       <c r="J42" s="31"/>
       <c r="K42" s="2"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="38"/>
+      <c r="M42" s="39"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -2551,7 +2554,7 @@
       <c r="J43" s="31"/>
       <c r="K43" s="2"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="38"/>
+      <c r="M43" s="39"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -2576,7 +2579,7 @@
       <c r="J44" s="31"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="38"/>
+      <c r="M44" s="39"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
@@ -2601,7 +2604,7 @@
       <c r="J45" s="31"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="38"/>
+      <c r="M45" s="39"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -2630,7 +2633,7 @@
         <v>52</v>
       </c>
       <c r="L46" s="2"/>
-      <c r="M46" s="38"/>
+      <c r="M46" s="39"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -2659,7 +2662,7 @@
         <v>53</v>
       </c>
       <c r="L47" s="2"/>
-      <c r="M47" s="38"/>
+      <c r="M47" s="39"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -2927,7 +2930,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="36" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -2956,7 +2959,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="2" t="s">
         <v>152</v>
       </c>
@@ -2983,7 +2986,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="35"/>
+      <c r="A61" s="36"/>
       <c r="B61" s="2" t="s">
         <v>153</v>
       </c>
@@ -3010,7 +3013,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="2" t="s">
         <v>154</v>
       </c>
@@ -3037,7 +3040,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="2" t="s">
         <v>155</v>
       </c>
@@ -3064,7 +3067,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
+      <c r="A64" s="36"/>
       <c r="B64" s="2" t="s">
         <v>280</v>
       </c>
@@ -3091,7 +3094,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
+      <c r="A65" s="36"/>
       <c r="B65" s="2" t="s">
         <v>156</v>
       </c>
@@ -3118,7 +3121,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="2" t="s">
         <v>161</v>
       </c>
@@ -3145,7 +3148,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="2" t="s">
         <v>162</v>
       </c>
@@ -3201,7 +3204,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="36" t="s">
         <v>168</v>
       </c>
       <c r="B69" t="s">
@@ -3230,7 +3233,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
+      <c r="A70" s="36"/>
       <c r="B70" t="s">
         <v>166</v>
       </c>
@@ -3257,7 +3260,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="35"/>
+      <c r="A71" s="36"/>
       <c r="B71" t="s">
         <v>167</v>
       </c>
@@ -3291,34 +3294,34 @@
       <c r="J72" s="24"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="37" t="s">
+      <c r="A73" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="37"/>
-      <c r="I73" s="37"/>
-      <c r="J73" s="37"/>
-      <c r="K73" s="37"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
     </row>
     <row r="74" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="36" t="s">
+      <c r="A74" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
-      <c r="K74" s="36"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
@@ -3691,8 +3694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3718,10 +3721,10 @@
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3733,8 +3736,8 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="39"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3744,10 +3747,10 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3757,8 +3760,8 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3789,11 +3792,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>62</v>
+      <c r="B8" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3801,12 +3807,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" t="s">
-        <v>277</v>
-      </c>
+      <c r="B9" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -3814,13 +3819,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>181</v>
+        <v>263</v>
+      </c>
+      <c r="D10" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3829,75 +3831,75 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="40"/>
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D12" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>276</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3945,7 +3947,7 @@
       <c r="C2" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="41" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3957,10 +3959,10 @@
       <c r="B3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -3970,8 +3972,8 @@
       <c r="B4" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
@@ -3981,8 +3983,8 @@
       <c r="B5" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
@@ -3995,7 +3997,7 @@
       <c r="C6" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>212</v>
       </c>
       <c r="E6" s="24"/>
@@ -4008,10 +4010,10 @@
       <c r="B7" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4022,8 +4024,8 @@
       <c r="B8" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4034,8 +4036,8 @@
       <c r="B9" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -4046,8 +4048,8 @@
       <c r="B10" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4058,8 +4060,8 @@
       <c r="B11" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4073,7 +4075,7 @@
       <c r="C12" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -4086,7 +4088,7 @@
       <c r="C13" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
@@ -4096,10 +4098,10 @@
       <c r="B14" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
@@ -4109,8 +4111,8 @@
       <c r="B15" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -4120,8 +4122,8 @@
       <c r="B16" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
@@ -4131,8 +4133,8 @@
       <c r="B17" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
     </row>
     <row r="18" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
@@ -4142,10 +4144,10 @@
       <c r="B18" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
@@ -4155,8 +4157,8 @@
       <c r="B19" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -4166,8 +4168,8 @@
       <c r="B20" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4177,8 +4179,8 @@
       <c r="B21" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4188,8 +4190,8 @@
       <c r="B22" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4199,10 +4201,10 @@
       <c r="B23" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4212,8 +4214,8 @@
       <c r="B24" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4223,10 +4225,10 @@
       <c r="B25" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4236,8 +4238,8 @@
       <c r="B26" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4247,8 +4249,8 @@
       <c r="B27" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -4258,8 +4260,8 @@
       <c r="B28" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4269,10 +4271,10 @@
       <c r="B29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="40"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4282,8 +4284,8 @@
       <c r="B30" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -4293,10 +4295,10 @@
       <c r="B31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="40"/>
+      <c r="D31" s="41"/>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -4306,8 +4308,8 @@
       <c r="B32" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4318,8 +4320,8 @@
       <c r="B33" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="24">
@@ -4329,10 +4331,10 @@
       <c r="B34" t="s">
         <v>146</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="40"/>
+      <c r="D34" s="41"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -4342,8 +4344,8 @@
       <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="40"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="41"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -4356,7 +4358,7 @@
       <c r="C36" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="40"/>
+      <c r="D36" s="41"/>
     </row>
     <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
@@ -4369,7 +4371,7 @@
       <c r="C37" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D37" s="40"/>
+      <c r="D37" s="41"/>
     </row>
     <row r="38" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
@@ -4382,7 +4384,7 @@
       <c r="C38" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="D38" s="40"/>
+      <c r="D38" s="41"/>
     </row>
     <row r="39" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
@@ -4392,10 +4394,10 @@
       <c r="B39" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="D39" s="40"/>
+      <c r="D39" s="41"/>
     </row>
     <row r="40" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
@@ -4405,8 +4407,8 @@
       <c r="B40" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
     </row>
     <row r="41" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
@@ -4416,10 +4418,10 @@
       <c r="B41" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="D41" s="40"/>
+      <c r="D41" s="41"/>
     </row>
     <row r="42" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
@@ -4429,8 +4431,8 @@
       <c r="B42" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
     </row>
     <row r="43" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
@@ -4440,8 +4442,8 @@
       <c r="B43" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
     </row>
     <row r="44" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
@@ -4454,7 +4456,7 @@
       <c r="C44" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D44" s="40"/>
+      <c r="D44" s="41"/>
     </row>
     <row r="45" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
@@ -4464,10 +4466,10 @@
       <c r="B45" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="41" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4479,8 +4481,8 @@
       <c r="B46" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
@@ -4490,10 +4492,10 @@
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C47" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="40"/>
+      <c r="D47" s="41"/>
     </row>
     <row r="48" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
@@ -4503,8 +4505,8 @@
       <c r="B48" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
@@ -4514,8 +4516,8 @@
       <c r="B49" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
@@ -4525,8 +4527,8 @@
       <c r="B50" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
@@ -4536,10 +4538,10 @@
       <c r="B51" t="s">
         <v>205</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="D51" s="40"/>
+      <c r="D51" s="41"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
@@ -4549,8 +4551,8 @@
       <c r="B52" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -4560,8 +4562,8 @@
       <c r="B53" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
@@ -4574,7 +4576,7 @@
       <c r="C54" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="D54" s="40"/>
+      <c r="D54" s="41"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
@@ -4587,7 +4589,7 @@
       <c r="C55" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="41" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4602,7 +4604,7 @@
       <c r="C56" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D56" s="40"/>
+      <c r="D56" s="41"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>

</xml_diff>

<commit_message>
split stuff out into headers
</commit_message>
<xml_diff>
--- a/CPU.xlsx
+++ b/CPU.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="275">
   <si>
     <t>Name</t>
   </si>
@@ -612,12 +612,6 @@
     <t>INT 1</t>
   </si>
   <si>
-    <t>MOV $R1,11</t>
-  </si>
-  <si>
-    <t>MOV NOP to R1</t>
-  </si>
-  <si>
     <t>Zero out the ENCREG MOVs</t>
   </si>
   <si>
@@ -651,9 +645,6 @@
     <t>Encryption = Off</t>
   </si>
   <si>
-    <t>Disable encryption</t>
-  </si>
-  <si>
     <t>MOV $ENCREG1,$R3</t>
   </si>
   <si>
@@ -678,9 +669,6 @@
     <t>Encrpyt with</t>
   </si>
   <si>
-    <t>Bootloader key 0xDEADBEEF</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -823,21 +811,6 @@
   </si>
   <si>
     <t>CMP32S</t>
-  </si>
-  <si>
-    <t>MOV [0],$R1</t>
-  </si>
-  <si>
-    <t>MOV [2],$R1</t>
-  </si>
-  <si>
-    <t>MOV [4],$R1</t>
-  </si>
-  <si>
-    <t>MOV [6],$R1</t>
-  </si>
-  <si>
-    <t>MOV [8],$R1</t>
   </si>
   <si>
     <t>MREGC</t>
@@ -893,13 +866,28 @@
     <t>ENCON; RETN</t>
   </si>
   <si>
-    <t>JNZ $ENCREG1,52</t>
-  </si>
-  <si>
-    <t>JNZ $ENCREG2,52</t>
-  </si>
-  <si>
     <t>Turn on ROM encryption and return</t>
+  </si>
+  <si>
+    <t>MOV [0],11</t>
+  </si>
+  <si>
+    <t>MOV [2],11</t>
+  </si>
+  <si>
+    <t>MOV [4],11</t>
+  </si>
+  <si>
+    <t>MOV [6],11</t>
+  </si>
+  <si>
+    <t>MOV [8],11</t>
+  </si>
+  <si>
+    <t>JNZ $ENCREG1,51</t>
+  </si>
+  <si>
+    <t>JNZ $ENCREG2,51</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1000,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1029,9 +1017,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1053,7 +1038,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1418,14 +1402,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="16"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
     <col min="5" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="59.7109375" customWidth="1"/>
     <col min="12" max="12" width="38.85546875" customWidth="1"/>
@@ -1442,8 +1426,8 @@
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>210</v>
+      <c r="D1" s="14" t="s">
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>20</v>
@@ -1451,10 +1435,10 @@
       <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1467,11 +1451,11 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="D2" s="19" t="str">
         <f>DEC2HEX(C2,2)</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -1479,10 +1463,10 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" t="s">
         <v>29</v>
       </c>
@@ -1496,11 +1480,11 @@
       </c>
       <c r="C3" s="2">
         <f>C2+1</f>
-        <v>2</v>
-      </c>
-      <c r="D3" s="21" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="str">
         <f t="shared" ref="D3:D70" si="0">DEC2HEX(C3,2)</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>18</v>
@@ -1508,10 +1492,10 @@
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1520,21 +1504,21 @@
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="22">
         <f>C3+1</f>
-        <v>3</v>
-      </c>
-      <c r="D4" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>03</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>02</v>
       </c>
       <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
       <c r="K4" t="s">
         <v>174</v>
       </c>
@@ -1545,19 +1529,19 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C72" si="1">C4+1</f>
-        <v>4</v>
-      </c>
-      <c r="D5" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>04</v>
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>03</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
       <c r="K5" t="s">
         <v>175</v>
       </c>
@@ -1571,19 +1555,19 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="D6" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>05</v>
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>04</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="2" t="s">
         <v>176</v>
       </c>
@@ -1597,19 +1581,19 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D7" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>06</v>
+        <v>5</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>05</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
       <c r="K7" s="2" t="s">
         <v>177</v>
       </c>
@@ -1620,16 +1604,16 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D8" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>07</v>
-      </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>06</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1640,11 +1624,11 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D9" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>08</v>
+        <v>7</v>
+      </c>
+      <c r="D9" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>07</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -1652,10 +1636,10 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
       <c r="K9" t="s">
         <v>30</v>
       </c>
@@ -1666,11 +1650,11 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="D10" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>09</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>08</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1678,10 +1662,10 @@
       <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
       <c r="K10" t="s">
         <v>31</v>
       </c>
@@ -1692,11 +1676,11 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="D11" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0A</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>09</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
@@ -1704,10 +1688,10 @@
       <c r="F11" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="K11" t="s">
         <v>32</v>
       </c>
@@ -1718,11 +1702,11 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="D12" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0B</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0A</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
@@ -1730,10 +1714,10 @@
       <c r="F12" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
       <c r="K12" t="s">
         <v>33</v>
       </c>
@@ -1744,11 +1728,11 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="D13" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0C</v>
+        <v>11</v>
+      </c>
+      <c r="D13" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0B</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1756,10 +1740,10 @@
       <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
       <c r="K13" t="s">
         <v>34</v>
       </c>
@@ -1770,11 +1754,11 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="D14" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0D</v>
+        <v>12</v>
+      </c>
+      <c r="D14" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0C</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -1782,25 +1766,25 @@
       <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
       <c r="K14" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="D15" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0E</v>
+        <v>13</v>
+      </c>
+      <c r="D15" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0D</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
@@ -1808,10 +1792,10 @@
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
       <c r="K15" s="5" t="s">
         <v>98</v>
       </c>
@@ -1822,11 +1806,11 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="D16" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>0F</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0E</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>18</v>
@@ -1834,10 +1818,10 @@
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
       <c r="K16" s="5" t="s">
         <v>99</v>
       </c>
@@ -1848,11 +1832,11 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="D17" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="D17" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>0F</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
@@ -1860,10 +1844,10 @@
       <c r="F17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
       <c r="K17" s="5" t="s">
         <v>158</v>
       </c>
@@ -1874,11 +1858,11 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="D18" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="D18" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>18</v>
@@ -1886,10 +1870,10 @@
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
       <c r="K18" s="5" t="s">
         <v>159</v>
       </c>
@@ -1903,11 +1887,11 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="D19" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D19" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
@@ -1915,10 +1899,10 @@
       <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
       <c r="K19" t="s">
         <v>35</v>
       </c>
@@ -1929,11 +1913,11 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="D20" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="D20" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
@@ -1941,10 +1925,10 @@
       <c r="F20" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
       <c r="K20" t="s">
         <v>36</v>
       </c>
@@ -1955,11 +1939,11 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="D21" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="D21" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
@@ -1967,10 +1951,10 @@
       <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
       <c r="K21" t="s">
         <v>37</v>
       </c>
@@ -1982,11 +1966,11 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D22" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="D22" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
@@ -1994,10 +1978,10 @@
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
       <c r="K22" s="2" t="s">
         <v>38</v>
       </c>
@@ -2011,11 +1995,11 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="D23" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="D23" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
@@ -2023,10 +2007,10 @@
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="2" t="s">
         <v>39</v>
       </c>
@@ -2040,11 +2024,11 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="D24" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="D24" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
@@ -2052,145 +2036,145 @@
       <c r="F24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
       <c r="K24" s="2" t="s">
         <v>40</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+    <row r="25" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" s="22">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="19" t="str">
+        <f t="shared" ref="D25:D27" si="2">DEC2HEX(C25,2)</f>
+        <v>17</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="C26" s="22">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="C25" s="24">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="D25" s="21" t="str">
-        <f t="shared" ref="D25:D27" si="2">DEC2HEX(C25,2)</f>
-        <v>18</v>
-      </c>
-      <c r="E25" s="24" t="s">
+      <c r="C27" s="22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D27" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F27" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="24" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="C26" s="24">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="D26" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="E26" s="24" t="s">
+    <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" s="22">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="E28" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F28" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-    </row>
-    <row r="27" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="C27" s="24">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="D27" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>1A</v>
-      </c>
-      <c r="E27" s="24" t="s">
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C29" s="22">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D29" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1B</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F29" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="24" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="C28" s="24">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="D28" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>1B</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-    </row>
-    <row r="29" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="C29" s="24">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="D29" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>1C</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="24" t="s">
-        <v>248</v>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="22" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2200,22 +2184,22 @@
       <c r="B30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="24">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="D30" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>1D</v>
-      </c>
-      <c r="E30" s="24" t="s">
+      <c r="C30" s="22">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1C</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="24"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="2" t="s">
         <v>54</v>
       </c>
@@ -2224,24 +2208,24 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="D31" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>1E</v>
+        <v>29</v>
+      </c>
+      <c r="D31" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1D</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
       <c r="K31" s="2"/>
       <c r="L31" s="4"/>
       <c r="M31" s="2"/>
@@ -2249,24 +2233,24 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="D32" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>1F</v>
+        <v>30</v>
+      </c>
+      <c r="D32" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1E</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
       <c r="K32" s="2"/>
       <c r="L32" s="4"/>
       <c r="M32" s="2"/>
@@ -2278,20 +2262,20 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="D33" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E33" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>1F</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="2"/>
       <c r="L33" s="4"/>
       <c r="M33" s="2"/>
@@ -2303,66 +2287,66 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="D34" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="E34" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="2"/>
       <c r="L34" s="4"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="C35" s="24">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D35" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="E35" s="24" t="s">
+    <row r="35" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C35" s="22">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="D35" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C36" s="24">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="D36" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>236</v>
+      </c>
+      <c r="C36" s="22">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D36" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -2374,22 +2358,22 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="D37" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="D37" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
       <c r="K37" s="2" t="s">
         <v>52</v>
       </c>
@@ -2403,22 +2387,22 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="D38" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="D38" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
       <c r="K38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2432,76 +2416,76 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="D39" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E39" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
       <c r="K39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="40" t="s">
+      <c r="M39" s="38" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="D40" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D40" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F40" s="2"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="40"/>
+      <c r="M40" s="38"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="D41" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="D41" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
       <c r="K41" s="2"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="40"/>
+      <c r="M41" s="38"/>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -2510,23 +2494,23 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="D42" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E42" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F42" s="2"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
       <c r="K42" s="2"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="40"/>
+      <c r="M42" s="38"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -2535,73 +2519,73 @@
       </c>
       <c r="C43" s="2">
         <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="D43" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2A</v>
-      </c>
-      <c r="E43" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E43" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="2"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
       <c r="K43" s="2"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="40"/>
+      <c r="M43" s="38"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="D44" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2B</v>
+        <v>42</v>
+      </c>
+      <c r="D44" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2A</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F44" s="2"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="40"/>
+      <c r="M44" s="38"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="D45" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2C</v>
+        <v>43</v>
+      </c>
+      <c r="D45" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2B</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F45" s="2"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="40"/>
+      <c r="M45" s="38"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
@@ -2610,27 +2594,27 @@
       </c>
       <c r="C46" s="2">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="D46" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2D</v>
+        <v>44</v>
+      </c>
+      <c r="D46" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2C</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
       <c r="K46" s="2" t="s">
         <v>52</v>
       </c>
       <c r="L46" s="2"/>
-      <c r="M46" s="40"/>
+      <c r="M46" s="38"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -2639,27 +2623,27 @@
       </c>
       <c r="C47" s="2">
         <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="D47" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2E</v>
+        <v>45</v>
+      </c>
+      <c r="D47" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2D</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
       <c r="K47" s="2" t="s">
         <v>53</v>
       </c>
       <c r="L47" s="2"/>
-      <c r="M47" s="40"/>
+      <c r="M47" s="38"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -2668,18 +2652,18 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="D48" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>2F</v>
+        <v>46</v>
+      </c>
+      <c r="D48" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2E</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
       <c r="K48" s="2" t="s">
         <v>61</v>
       </c>
@@ -2695,22 +2679,22 @@
       </c>
       <c r="C49" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="D49" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="E49" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>2F</v>
+      </c>
+      <c r="E49" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="31"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
       <c r="K49" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
@@ -2722,22 +2706,22 @@
       </c>
       <c r="C50" s="2">
         <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="D50" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="E50" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E50" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F50" s="24"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
       <c r="K50" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
@@ -2749,18 +2733,18 @@
       </c>
       <c r="C51" s="2">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="D51" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="D51" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
       <c r="K51" s="2" t="s">
         <v>121</v>
       </c>
@@ -2774,18 +2758,18 @@
       </c>
       <c r="C52" s="2">
         <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="D52" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <v>50</v>
+      </c>
+      <c r="D52" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
       <c r="K52" s="2" t="s">
         <v>116</v>
       </c>
@@ -2799,118 +2783,118 @@
       </c>
       <c r="C53" s="2">
         <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="D53" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <v>51</v>
+      </c>
+      <c r="D53" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
       <c r="K53" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
+    <row r="54" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" s="15">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="D54" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C54" s="16">
+    </row>
+    <row r="55" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="15">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="D54" s="21" t="str">
+      <c r="D55" s="19" t="str">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="16" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="16" t="s">
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C55" s="16">
+    </row>
+    <row r="56" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="17">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="D55" s="21" t="str">
+      <c r="D56" s="19" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C56" s="19">
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C57" s="17">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="D56" s="21" t="str">
+      <c r="D57" s="19" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
-      <c r="K56" s="19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="C57" s="19">
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="C58" s="22">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="D57" s="21" t="str">
+      <c r="D58" s="19" t="str">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="19" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="C58" s="24">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="D58" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="K58" s="24" t="s">
-        <v>275</v>
+      <c r="K58" s="22" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -2920,13 +2904,13 @@
       <c r="B59" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C59" s="24">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="D59" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3A</v>
+      <c r="C59" s="22">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="D59" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>18</v>
@@ -2934,16 +2918,16 @@
       <c r="F59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
       <c r="K59" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="35" t="s">
         <v>167</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2951,11 +2935,11 @@
       </c>
       <c r="C60" s="2">
         <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="D60" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3B</v>
+        <v>58</v>
+      </c>
+      <c r="D60" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3A</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>18</v>
@@ -2963,26 +2947,26 @@
       <c r="F60" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
       <c r="K60" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="37"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="2" t="s">
         <v>151</v>
       </c>
       <c r="C61" s="2">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D61" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3C</v>
+        <v>59</v>
+      </c>
+      <c r="D61" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>18</v>
@@ -2990,26 +2974,26 @@
       <c r="F61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-      <c r="J61" s="31"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
       <c r="K61" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="37"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C62" s="2">
         <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="D62" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3D</v>
+        <v>60</v>
+      </c>
+      <c r="D62" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>18</v>
@@ -3017,26 +3001,26 @@
       <c r="F62" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
       <c r="K62" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="D63" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3E</v>
+        <v>61</v>
+      </c>
+      <c r="D63" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3D</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>18</v>
@@ -3044,26 +3028,26 @@
       <c r="F63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="31"/>
-      <c r="J63" s="31"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
       <c r="K63" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
+      <c r="A64" s="35"/>
       <c r="B64" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="D64" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>3F</v>
+        <v>62</v>
+      </c>
+      <c r="D64" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3E</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>18</v>
@@ -3071,26 +3055,26 @@
       <c r="F64" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
       <c r="K64" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="D65" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <v>63</v>
+      </c>
+      <c r="D65" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>3F</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>18</v>
@@ -3098,26 +3082,26 @@
       <c r="F65" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G65" s="31"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="29"/>
       <c r="K65" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C66" s="2">
         <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="D66" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <v>64</v>
+      </c>
+      <c r="D66" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>18</v>
@@ -3125,26 +3109,26 @@
       <c r="F66" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
       <c r="K66" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
+      <c r="A67" s="35"/>
       <c r="B67" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C67" s="2">
         <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="D67" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <v>65</v>
+      </c>
+      <c r="D67" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>18</v>
@@ -3152,26 +3136,26 @@
       <c r="F67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G67" s="31"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="31"/>
-      <c r="J67" s="31"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="29"/>
       <c r="K67" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C68" s="2">
         <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="D68" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="D68" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>18</v>
@@ -3179,10 +3163,10 @@
       <c r="F68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G68" s="31"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="31"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
       <c r="K68" s="5" t="s">
         <v>159</v>
       </c>
@@ -3196,11 +3180,11 @@
       </c>
       <c r="C69" s="2">
         <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="D69" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="D69" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>18</v>
@@ -3208,16 +3192,16 @@
       <c r="F69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G69" s="31"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
       <c r="K69" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="35" t="s">
         <v>167</v>
       </c>
       <c r="B70" t="s">
@@ -3225,11 +3209,11 @@
       </c>
       <c r="C70" s="2">
         <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="D70" s="21" t="str">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="D70" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>18</v>
@@ -3237,26 +3221,26 @@
       <c r="F70" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
       <c r="K70" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="37"/>
+      <c r="A71" s="35"/>
       <c r="B71" t="s">
         <v>165</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="D71" s="21" t="str">
+        <v>69</v>
+      </c>
+      <c r="D71" s="19" t="str">
         <f t="shared" ref="D71:D72" si="3">DEC2HEX(C71,2)</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>18</v>
@@ -3264,26 +3248,26 @@
       <c r="F71" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
       <c r="K71" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="37"/>
+      <c r="A72" s="35"/>
       <c r="B72" t="s">
         <v>166</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="D72" s="21" t="str">
+        <v>70</v>
+      </c>
+      <c r="D72" s="19" t="str">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>18</v>
@@ -3291,62 +3275,62 @@
       <c r="F72" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
       <c r="K72" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
-      <c r="J73" s="24"/>
+      <c r="A73" s="12"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="39"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
     </row>
     <row r="75" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
+      <c r="A75" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B75" s="38"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+      <c r="A76" s="12"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
+      <c r="A77" s="12"/>
     </row>
     <row r="78" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+      <c r="A78" s="12"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3520,7 +3504,7 @@
         <v>181</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>79</v>
@@ -3535,7 +3519,7 @@
         <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D12" t="s">
         <v>79</v>
@@ -3581,34 +3565,34 @@
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="21" customWidth="1"/>
     <col min="9" max="9" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>217</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3616,86 +3600,86 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="G2" s="25"/>
-      <c r="I2" s="28" t="s">
-        <v>222</v>
+      <c r="G2" s="23"/>
+      <c r="I2" s="26" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="21">
         <f t="shared" ref="A3:A6" si="0">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="I3" s="27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="I4" s="28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="I3" s="29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="I4" s="30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="25" t="s">
-        <v>225</v>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G6" s="25"/>
+        <v>229</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3734,10 +3718,10 @@
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3749,8 +3733,8 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3760,10 +3744,10 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="42"/>
+      <c r="C4" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3773,8 +3757,8 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3805,13 +3789,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3820,11 +3804,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -3832,10 +3816,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,7 +3860,7 @@
       <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="22" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3886,10 +3870,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D16" t="s">
         <v>254</v>
-      </c>
-      <c r="D16" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3898,10 +3882,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,10 +3905,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3936,7 +3920,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3945,244 +3929,234 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
-        <f>1</f>
+      <c r="D1" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <f t="shared" ref="A3:A19" si="0">A2+1</f>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <f t="shared" ref="A3:A17" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="41"/>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+    </row>
+    <row r="4" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="B4" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="E6" s="24"/>
+      <c r="B6" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="B7" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="B9" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="B10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="B11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="B12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="41"/>
-    </row>
-    <row r="14" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="B13" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="41"/>
-    </row>
-    <row r="15" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="B14" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="B15" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="B16" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="39"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-    </row>
-    <row r="18" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
-        <f t="shared" si="0"/>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <f t="shared" ref="A18:A51" si="1">A17+1</f>
         <v>17</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="41"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="41"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" ref="A20:A53" si="1">A19+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="41"/>
+        <v>184</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="39"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -4190,10 +4164,12 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="41"/>
+        <v>105</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -4201,10 +4177,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="41"/>
+        <v>106</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -4212,12 +4188,12 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="41"/>
+        <v>102</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -4225,10 +4201,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
+        <v>107</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4236,12 +4212,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="41"/>
+        <v>108</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4249,32 +4223,34 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>185</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
+      <c r="B28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -4282,12 +4258,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="41"/>
+        <v>143</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -4295,10 +4271,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
+        <v>259</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -4306,325 +4283,300 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="41"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+        <v>119</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>119</v>
+      <c r="B33" t="s">
+        <v>113</v>
       </c>
       <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
+      <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24">
+      <c r="A34" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="41"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="B34" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="39"/>
+    </row>
+    <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="41"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="B35" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="39"/>
+    </row>
+    <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D36" s="41"/>
-    </row>
-    <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16">
+      <c r="B36" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="39"/>
+    </row>
+    <row r="37" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C37" s="17" t="s">
+      <c r="B37" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="D37" s="39"/>
+    </row>
+    <row r="38" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+    </row>
+    <row r="39" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="D39" s="39"/>
+    </row>
+    <row r="40" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41" s="39"/>
+    </row>
+    <row r="42" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="D37" s="41"/>
-    </row>
-    <row r="38" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="C38" s="20" t="s">
+      <c r="D42" s="39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="39"/>
+    </row>
+    <row r="45" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+    </row>
+    <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="39"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="D38" s="41"/>
-    </row>
-    <row r="39" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="D39" s="41"/>
-    </row>
-    <row r="40" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-    </row>
-    <row r="41" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C41" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="D41" s="41"/>
-    </row>
-    <row r="42" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-    </row>
-    <row r="43" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="D43" s="41"/>
-    </row>
-    <row r="44" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="C44" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="41"/>
-    </row>
-    <row r="47" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-    </row>
-    <row r="48" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="16">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>276</v>
-      </c>
-      <c r="C50" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="D50" s="41"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="16">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
+      <c r="D51" s="39"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="16">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
+      <c r="A52" s="15"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="34"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>274</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="D53" s="41"/>
+      <c r="A53" s="21"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="34"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="36"/>
+      <c r="A54" s="15"/>
+      <c r="C54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="16"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="36"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="C56" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" s="17"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+      <c r="A55" s="15"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D44:D53"/>
-    <mergeCell ref="D6:D43"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="D5:D41"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D2:D4"/>
     <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C27:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4649,13 +4601,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>126</v>
       </c>
       <c r="B2" t="s">
@@ -4663,12 +4615,12 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B4" t="s">
@@ -4677,13 +4629,13 @@
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>117</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>128</v>
       </c>
       <c r="B6" t="s">
@@ -4692,12 +4644,12 @@
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B8" t="s">
@@ -4705,7 +4657,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gitignore excel temps. also add add files. also base for I/O
</commit_message>
<xml_diff>
--- a/CPU.xlsx
+++ b/CPU.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22725" windowHeight="12495" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="275">
   <si>
     <t>Name</t>
   </si>
@@ -1402,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3350,7 +3350,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3553,8 +3553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3660,7 +3660,9 @@
         <v>221</v>
       </c>
       <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="F5" s="23" t="s">
+        <v>221</v>
+      </c>
       <c r="G5" s="23" t="s">
         <v>221</v>
       </c>
@@ -4560,11 +4562,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="D5:D41"/>
-    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="C42:C43"/>
@@ -4577,6 +4574,11 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="D5:D41"/>
+    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>